<commit_message>
add freeRTOSv9.0.0 source code
</commit_message>
<xml_diff>
--- a/工程目录.xlsx
+++ b/工程目录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\STM32_WS\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BCC23E-1FC7-42CA-8881-3F2F71DB2AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43927CF-EC03-4658-9576-3CDA17CACD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Template_Project</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,6 +64,14 @@
   </si>
   <si>
     <t>STM32 跑马灯样例工程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FreeRTOSv9.0.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FreeRTOS 9.0.0 源码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -415,7 +423,7 @@
   <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -465,8 +473,12 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>

</xml_diff>

<commit_message>
add FreeRTOSv202112.00 source code
</commit_message>
<xml_diff>
--- a/工程目录.xlsx
+++ b/工程目录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\STM32_WS\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43927CF-EC03-4658-9576-3CDA17CACD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE57D8BC-5D5D-4C6C-9044-75299FE404A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Template_Project</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +72,14 @@
   </si>
   <si>
     <t>FreeRTOS 9.0.0 源码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FreeRTOSv202112.00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FreeRTOSv202112.00 源码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -423,7 +431,7 @@
   <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -481,8 +489,12 @@
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>

</xml_diff>